<commit_message>
product edit and delete functionality
</commit_message>
<xml_diff>
--- a/flask_project/data/awae_products.xlsx
+++ b/flask_project/data/awae_products.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HDD documents\University\comp3900\capstone-project-3900-h10a-awae\flask_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD9922A-8142-4A06-B9E5-DC5E5A048F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA368B2D-FA45-4696-81CB-F9E72BBFF948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15612" yWindow="3432" windowWidth="18780" windowHeight="11976" xr2:uid="{D399C2E0-3F7A-4710-BFC9-FE24D65D8127}"/>
+    <workbookView xWindow="2064" yWindow="3576" windowWidth="18780" windowHeight="11976" xr2:uid="{D399C2E0-3F7A-4710-BFC9-FE24D65D8127}"/>
   </bookViews>
   <sheets>
     <sheet name="All Products" sheetId="1" r:id="rId1"/>
-    <sheet name="Coffee" sheetId="2" r:id="rId2"/>
-    <sheet name="Alt Milk" sheetId="3" r:id="rId3"/>
-    <sheet name="Meal Kit" sheetId="4" r:id="rId4"/>
-    <sheet name="Dessert Kit" sheetId="5" r:id="rId5"/>
-    <sheet name="Tools" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
+    <sheet name="Coffee" sheetId="2" r:id="rId3"/>
+    <sheet name="Alt Milk" sheetId="3" r:id="rId4"/>
+    <sheet name="Meal Kit" sheetId="4" r:id="rId5"/>
+    <sheet name="Dessert Kit" sheetId="5" r:id="rId6"/>
+    <sheet name="Tools" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All Products'!$A$1:$H$112</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All Products'!$A$1:$G$112</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1330,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4689175-1BCB-4AC3-A0ED-0BD6571DC856}">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J58" sqref="J58"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1345,12 +1346,11 @@
     <col min="5" max="5" width="85.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.5546875" customWidth="1"/>
     <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.109375" customWidth="1"/>
-    <col min="10" max="10" width="28.6640625" customWidth="1"/>
+    <col min="8" max="8" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1373,16 +1373,13 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I1" t="s">
-        <v>229</v>
-      </c>
-      <c r="J1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="83.4" customHeight="1">
+    <row r="2" spans="1:9" ht="83.4" customHeight="1">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1404,17 +1401,14 @@
       <c r="G2">
         <v>2</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2">
-        <v>100</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="57.6">
+    <row r="3" spans="1:9" ht="57.6">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1436,17 +1430,14 @@
       <c r="G3">
         <v>2</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3">
-        <v>100</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="H3">
+        <v>100</v>
+      </c>
+      <c r="I3" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="72">
+    <row r="4" spans="1:9" ht="57.6">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1468,17 +1459,14 @@
       <c r="G4">
         <v>2</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4">
-        <v>100</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="H4">
+        <v>100</v>
+      </c>
+      <c r="I4" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="28.8">
+    <row r="5" spans="1:9" ht="28.8">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1500,17 +1488,14 @@
       <c r="G5">
         <v>2</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5">
-        <v>100</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="H5">
+        <v>100</v>
+      </c>
+      <c r="I5" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="28.8">
+    <row r="6" spans="1:9" ht="28.8">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1532,17 +1517,14 @@
       <c r="G6">
         <v>2</v>
       </c>
-      <c r="H6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6">
-        <v>100</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="I6" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="57.6">
+    <row r="7" spans="1:9" ht="43.2">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1564,17 +1546,14 @@
       <c r="G7">
         <v>2</v>
       </c>
-      <c r="H7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7">
-        <v>100</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="H7">
+        <v>100</v>
+      </c>
+      <c r="I7" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="43.2">
+    <row r="8" spans="1:9" ht="43.2">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1596,17 +1575,14 @@
       <c r="G8">
         <v>2</v>
       </c>
-      <c r="H8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8">
-        <v>100</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="H8">
+        <v>100</v>
+      </c>
+      <c r="I8" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="57.6">
+    <row r="9" spans="1:9" ht="57.6">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -1628,17 +1604,14 @@
       <c r="G9">
         <v>2</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9">
-        <v>100</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="H9">
+        <v>100</v>
+      </c>
+      <c r="I9" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="43.2">
+    <row r="10" spans="1:9" ht="43.2">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1660,17 +1633,14 @@
       <c r="G10">
         <v>2</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10">
-        <v>100</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="H10">
+        <v>100</v>
+      </c>
+      <c r="I10" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="25.8">
+    <row r="11" spans="1:9" ht="25.8">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -1692,17 +1662,14 @@
       <c r="G11">
         <v>2</v>
       </c>
-      <c r="H11" t="s">
-        <v>62</v>
-      </c>
-      <c r="I11">
-        <v>100</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="H11">
+        <v>100</v>
+      </c>
+      <c r="I11" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="43.2">
+    <row r="12" spans="1:9" ht="43.2">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -1724,17 +1691,14 @@
       <c r="G12">
         <v>2</v>
       </c>
-      <c r="H12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I12">
-        <v>100</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="H12">
+        <v>100</v>
+      </c>
+      <c r="I12" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2">
+    <row r="13" spans="1:9" ht="43.2">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -1756,17 +1720,14 @@
       <c r="G13">
         <v>2</v>
       </c>
-      <c r="H13" t="s">
-        <v>70</v>
-      </c>
-      <c r="I13">
-        <v>100</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="H13">
+        <v>100</v>
+      </c>
+      <c r="I13" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="43.2">
+    <row r="14" spans="1:9" ht="43.2">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1788,17 +1749,14 @@
       <c r="G14">
         <v>2</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I14">
-        <v>100</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="H14">
+        <v>100</v>
+      </c>
+      <c r="I14" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="57.6">
+    <row r="15" spans="1:9" ht="57.6">
       <c r="A15" t="s">
         <v>78</v>
       </c>
@@ -1820,17 +1778,14 @@
       <c r="G15">
         <v>2</v>
       </c>
-      <c r="H15" t="s">
-        <v>80</v>
-      </c>
-      <c r="I15">
-        <v>100</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="H15">
+        <v>100</v>
+      </c>
+      <c r="I15" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="28.8">
+    <row r="16" spans="1:9" ht="28.8">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -1852,17 +1807,14 @@
       <c r="G16">
         <v>2</v>
       </c>
-      <c r="H16" t="s">
-        <v>83</v>
-      </c>
-      <c r="I16">
-        <v>100</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="H16">
+        <v>100</v>
+      </c>
+      <c r="I16" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="28.8">
+    <row r="17" spans="1:9" ht="28.8">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -1884,17 +1836,14 @@
       <c r="G17">
         <v>2</v>
       </c>
-      <c r="H17" t="s">
-        <v>87</v>
-      </c>
-      <c r="I17">
-        <v>100</v>
-      </c>
-      <c r="J17" t="s">
+      <c r="H17">
+        <v>100</v>
+      </c>
+      <c r="I17" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="28.8">
+    <row r="18" spans="1:9" ht="28.8">
       <c r="A18" t="s">
         <v>90</v>
       </c>
@@ -1916,17 +1865,14 @@
       <c r="G18">
         <v>2</v>
       </c>
-      <c r="H18" t="s">
-        <v>92</v>
-      </c>
-      <c r="I18">
-        <v>100</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="H18">
+        <v>100</v>
+      </c>
+      <c r="I18" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="57.6">
+    <row r="19" spans="1:9" ht="57.6">
       <c r="A19" t="s">
         <v>95</v>
       </c>
@@ -1948,17 +1894,14 @@
       <c r="G19">
         <v>2</v>
       </c>
-      <c r="H19" t="s">
-        <v>99</v>
-      </c>
-      <c r="I19">
-        <v>100</v>
-      </c>
-      <c r="J19" t="s">
+      <c r="H19">
+        <v>100</v>
+      </c>
+      <c r="I19" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="129.6">
+    <row r="20" spans="1:9" ht="129.6">
       <c r="A20" t="s">
         <v>103</v>
       </c>
@@ -1980,17 +1923,14 @@
       <c r="G20">
         <v>2</v>
       </c>
-      <c r="H20" t="s">
-        <v>105</v>
-      </c>
-      <c r="I20">
-        <v>100</v>
-      </c>
-      <c r="J20" t="s">
+      <c r="H20">
+        <v>100</v>
+      </c>
+      <c r="I20" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="129.6">
+    <row r="21" spans="1:9" ht="129.6">
       <c r="A21" t="s">
         <v>107</v>
       </c>
@@ -2012,17 +1952,14 @@
       <c r="G21">
         <v>2</v>
       </c>
-      <c r="H21" t="s">
-        <v>108</v>
-      </c>
-      <c r="I21">
-        <v>100</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="H21">
+        <v>100</v>
+      </c>
+      <c r="I21" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="129.6">
+    <row r="22" spans="1:9" ht="129.6">
       <c r="A22" t="s">
         <v>111</v>
       </c>
@@ -2044,17 +1981,14 @@
       <c r="G22">
         <v>2</v>
       </c>
-      <c r="H22" t="s">
-        <v>112</v>
-      </c>
-      <c r="I22">
-        <v>100</v>
-      </c>
-      <c r="J22" t="s">
+      <c r="H22">
+        <v>100</v>
+      </c>
+      <c r="I22" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="100.8">
+    <row r="23" spans="1:9" ht="100.8">
       <c r="A23" t="s">
         <v>113</v>
       </c>
@@ -2076,17 +2010,14 @@
       <c r="G23">
         <v>2</v>
       </c>
-      <c r="H23" t="s">
-        <v>116</v>
-      </c>
-      <c r="I23">
-        <v>100</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="H23">
+        <v>100</v>
+      </c>
+      <c r="I23" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="43.2">
+    <row r="24" spans="1:9" ht="43.2">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -2108,17 +2039,14 @@
       <c r="G24">
         <v>2</v>
       </c>
-      <c r="H24" t="s">
-        <v>119</v>
-      </c>
-      <c r="I24">
-        <v>100</v>
-      </c>
-      <c r="J24" t="s">
+      <c r="H24">
+        <v>100</v>
+      </c>
+      <c r="I24" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="28.8">
+    <row r="25" spans="1:9" ht="28.8">
       <c r="A25" t="s">
         <v>124</v>
       </c>
@@ -2140,17 +2068,14 @@
       <c r="G25">
         <v>2</v>
       </c>
-      <c r="H25" t="s">
-        <v>123</v>
-      </c>
-      <c r="I25">
-        <v>100</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="H25">
+        <v>100</v>
+      </c>
+      <c r="I25" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="28.8">
+    <row r="26" spans="1:9" ht="28.8">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -2172,17 +2097,14 @@
       <c r="G26">
         <v>2</v>
       </c>
-      <c r="H26" t="s">
-        <v>126</v>
-      </c>
-      <c r="I26">
-        <v>100</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="H26">
+        <v>100</v>
+      </c>
+      <c r="I26" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="28.8">
+    <row r="27" spans="1:9" ht="28.8">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -2204,17 +2126,14 @@
       <c r="G27">
         <v>2</v>
       </c>
-      <c r="H27" t="s">
-        <v>129</v>
-      </c>
-      <c r="I27">
-        <v>100</v>
-      </c>
-      <c r="J27" t="s">
+      <c r="H27">
+        <v>100</v>
+      </c>
+      <c r="I27" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="57.6">
+    <row r="28" spans="1:9" ht="57.6">
       <c r="A28" t="s">
         <v>130</v>
       </c>
@@ -2236,17 +2155,14 @@
       <c r="G28">
         <v>2</v>
       </c>
-      <c r="H28" t="s">
-        <v>134</v>
-      </c>
-      <c r="I28">
-        <v>100</v>
-      </c>
-      <c r="J28" t="s">
+      <c r="H28">
+        <v>100</v>
+      </c>
+      <c r="I28" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="85.8" customHeight="1">
+    <row r="29" spans="1:9" ht="85.8" customHeight="1">
       <c r="A29" t="s">
         <v>136</v>
       </c>
@@ -2268,17 +2184,14 @@
       <c r="G29">
         <v>2</v>
       </c>
-      <c r="H29" t="s">
-        <v>138</v>
-      </c>
-      <c r="I29">
-        <v>100</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="H29">
+        <v>100</v>
+      </c>
+      <c r="I29" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="28.8">
+    <row r="30" spans="1:9" ht="28.8">
       <c r="A30" t="s">
         <v>139</v>
       </c>
@@ -2300,14 +2213,14 @@
       <c r="G30">
         <v>2</v>
       </c>
-      <c r="I30">
-        <v>100</v>
-      </c>
-      <c r="J30" t="s">
+      <c r="H30">
+        <v>100</v>
+      </c>
+      <c r="I30" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="43.2">
+    <row r="31" spans="1:9" ht="43.2">
       <c r="A31" t="s">
         <v>142</v>
       </c>
@@ -2329,17 +2242,14 @@
       <c r="G31">
         <v>2</v>
       </c>
-      <c r="H31" t="s">
-        <v>144</v>
-      </c>
-      <c r="I31">
-        <v>100</v>
-      </c>
-      <c r="J31" t="s">
+      <c r="H31">
+        <v>100</v>
+      </c>
+      <c r="I31" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>146</v>
       </c>
@@ -2361,17 +2271,14 @@
       <c r="G32">
         <v>2</v>
       </c>
-      <c r="H32" t="s">
-        <v>147</v>
-      </c>
-      <c r="I32">
-        <v>100</v>
-      </c>
-      <c r="J32" t="s">
+      <c r="H32">
+        <v>100</v>
+      </c>
+      <c r="I32" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>149</v>
       </c>
@@ -2393,17 +2300,14 @@
       <c r="G33">
         <v>2</v>
       </c>
-      <c r="H33" t="s">
-        <v>150</v>
-      </c>
-      <c r="I33">
-        <v>100</v>
-      </c>
-      <c r="J33" t="s">
+      <c r="H33">
+        <v>100</v>
+      </c>
+      <c r="I33" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>152</v>
       </c>
@@ -2425,17 +2329,14 @@
       <c r="G34">
         <v>2</v>
       </c>
-      <c r="H34" t="s">
-        <v>154</v>
-      </c>
-      <c r="I34">
-        <v>100</v>
-      </c>
-      <c r="J34" t="s">
+      <c r="H34">
+        <v>100</v>
+      </c>
+      <c r="I34" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>155</v>
       </c>
@@ -2457,17 +2358,14 @@
       <c r="G35">
         <v>2</v>
       </c>
-      <c r="H35" t="s">
-        <v>158</v>
-      </c>
-      <c r="I35">
-        <v>100</v>
-      </c>
-      <c r="J35" t="s">
+      <c r="H35">
+        <v>100</v>
+      </c>
+      <c r="I35" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="43.2">
+    <row r="36" spans="1:9" ht="43.2">
       <c r="A36" t="s">
         <v>161</v>
       </c>
@@ -2489,17 +2387,14 @@
       <c r="G36">
         <v>2</v>
       </c>
-      <c r="H36" t="s">
-        <v>162</v>
-      </c>
-      <c r="I36">
-        <v>100</v>
-      </c>
-      <c r="J36" t="s">
+      <c r="H36">
+        <v>100</v>
+      </c>
+      <c r="I36" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="43.2">
+    <row r="37" spans="1:9" ht="43.2">
       <c r="A37" t="s">
         <v>163</v>
       </c>
@@ -2521,17 +2416,14 @@
       <c r="G37">
         <v>2</v>
       </c>
-      <c r="H37" t="s">
-        <v>167</v>
-      </c>
-      <c r="I37">
-        <v>100</v>
-      </c>
-      <c r="J37" t="s">
+      <c r="H37">
+        <v>100</v>
+      </c>
+      <c r="I37" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="43.2">
+    <row r="38" spans="1:9" ht="43.2">
       <c r="A38" t="s">
         <v>168</v>
       </c>
@@ -2553,17 +2445,14 @@
       <c r="G38">
         <v>2</v>
       </c>
-      <c r="H38" t="s">
-        <v>170</v>
-      </c>
-      <c r="I38">
-        <v>100</v>
-      </c>
-      <c r="J38" t="s">
+      <c r="H38">
+        <v>100</v>
+      </c>
+      <c r="I38" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="28.8">
+    <row r="39" spans="1:9" ht="28.8">
       <c r="A39" t="s">
         <v>171</v>
       </c>
@@ -2585,17 +2474,14 @@
       <c r="G39">
         <v>2</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="I39">
-        <v>100</v>
-      </c>
-      <c r="J39" t="s">
+      <c r="H39">
+        <v>100</v>
+      </c>
+      <c r="I39" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="100.8">
+    <row r="40" spans="1:9" ht="100.8">
       <c r="A40" t="s">
         <v>174</v>
       </c>
@@ -2617,17 +2503,14 @@
       <c r="G40">
         <v>2</v>
       </c>
-      <c r="H40" t="s">
-        <v>177</v>
-      </c>
-      <c r="I40">
-        <v>100</v>
-      </c>
-      <c r="J40" t="s">
+      <c r="H40">
+        <v>100</v>
+      </c>
+      <c r="I40" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="43.2">
+    <row r="41" spans="1:9" ht="43.2">
       <c r="A41" t="s">
         <v>178</v>
       </c>
@@ -2649,17 +2532,14 @@
       <c r="G41">
         <v>2</v>
       </c>
-      <c r="H41" t="s">
-        <v>180</v>
-      </c>
-      <c r="I41">
-        <v>100</v>
-      </c>
-      <c r="J41" t="s">
+      <c r="H41">
+        <v>100</v>
+      </c>
+      <c r="I41" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="43.2">
+    <row r="42" spans="1:9" ht="43.2">
       <c r="A42" t="s">
         <v>181</v>
       </c>
@@ -2681,17 +2561,14 @@
       <c r="G42">
         <v>2</v>
       </c>
-      <c r="H42" t="s">
-        <v>184</v>
-      </c>
-      <c r="I42">
-        <v>100</v>
-      </c>
-      <c r="J42" t="s">
+      <c r="H42">
+        <v>100</v>
+      </c>
+      <c r="I42" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="57.6">
+    <row r="43" spans="1:9" ht="57.6">
       <c r="A43" t="s">
         <v>185</v>
       </c>
@@ -2713,17 +2590,14 @@
       <c r="G43">
         <v>2</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="I43">
-        <v>100</v>
-      </c>
-      <c r="J43" t="s">
+      <c r="H43">
+        <v>100</v>
+      </c>
+      <c r="I43" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="72">
+    <row r="44" spans="1:9" ht="72">
       <c r="A44" t="s">
         <v>189</v>
       </c>
@@ -2745,17 +2619,14 @@
       <c r="G44">
         <v>2</v>
       </c>
-      <c r="H44" t="s">
-        <v>192</v>
-      </c>
-      <c r="I44">
-        <v>100</v>
-      </c>
-      <c r="J44" t="s">
+      <c r="H44">
+        <v>100</v>
+      </c>
+      <c r="I44" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="57.6">
+    <row r="45" spans="1:9" ht="57.6">
       <c r="A45" t="s">
         <v>193</v>
       </c>
@@ -2777,17 +2648,14 @@
       <c r="G45">
         <v>2</v>
       </c>
-      <c r="H45" t="s">
-        <v>196</v>
-      </c>
-      <c r="I45">
-        <v>100</v>
-      </c>
-      <c r="J45" t="s">
+      <c r="H45">
+        <v>100</v>
+      </c>
+      <c r="I45" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="43.2">
+    <row r="46" spans="1:9" ht="43.2">
       <c r="A46" t="s">
         <v>197</v>
       </c>
@@ -2809,17 +2677,14 @@
       <c r="G46">
         <v>2</v>
       </c>
-      <c r="H46" t="s">
-        <v>200</v>
-      </c>
-      <c r="I46">
-        <v>100</v>
-      </c>
-      <c r="J46" t="s">
+      <c r="H46">
+        <v>100</v>
+      </c>
+      <c r="I46" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="57.6">
+    <row r="47" spans="1:9" ht="57.6">
       <c r="A47" t="s">
         <v>201</v>
       </c>
@@ -2841,17 +2706,14 @@
       <c r="G47">
         <v>2</v>
       </c>
-      <c r="H47" t="s">
-        <v>204</v>
-      </c>
-      <c r="I47">
-        <v>100</v>
-      </c>
-      <c r="J47" t="s">
+      <c r="H47">
+        <v>100</v>
+      </c>
+      <c r="I47" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="28.8">
+    <row r="48" spans="1:9" ht="28.8">
       <c r="A48" t="s">
         <v>205</v>
       </c>
@@ -2873,17 +2735,14 @@
       <c r="G48">
         <v>2</v>
       </c>
-      <c r="H48" t="s">
-        <v>208</v>
-      </c>
-      <c r="I48">
-        <v>100</v>
-      </c>
-      <c r="J48" t="s">
+      <c r="H48">
+        <v>100</v>
+      </c>
+      <c r="I48" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>209</v>
       </c>
@@ -2905,17 +2764,14 @@
       <c r="G49">
         <v>2</v>
       </c>
-      <c r="H49" t="s">
-        <v>208</v>
-      </c>
-      <c r="I49">
-        <v>100</v>
-      </c>
-      <c r="J49" t="s">
+      <c r="H49">
+        <v>100</v>
+      </c>
+      <c r="I49" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="28.8">
+    <row r="50" spans="1:9" ht="28.8">
       <c r="A50" t="s">
         <v>211</v>
       </c>
@@ -2937,17 +2793,14 @@
       <c r="G50">
         <v>2</v>
       </c>
-      <c r="H50" t="s">
-        <v>208</v>
-      </c>
-      <c r="I50">
-        <v>100</v>
-      </c>
-      <c r="J50" t="s">
+      <c r="H50">
+        <v>100</v>
+      </c>
+      <c r="I50" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>213</v>
       </c>
@@ -2969,17 +2822,14 @@
       <c r="G51">
         <v>2</v>
       </c>
-      <c r="H51" t="s">
-        <v>208</v>
-      </c>
-      <c r="I51">
-        <v>100</v>
-      </c>
-      <c r="J51" t="s">
+      <c r="H51">
+        <v>100</v>
+      </c>
+      <c r="I51" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="28.8">
+    <row r="52" spans="1:9" ht="28.8">
       <c r="A52" t="s">
         <v>216</v>
       </c>
@@ -3001,17 +2851,14 @@
       <c r="G52">
         <v>2</v>
       </c>
-      <c r="H52" t="s">
-        <v>219</v>
-      </c>
-      <c r="I52">
-        <v>100</v>
-      </c>
-      <c r="J52" t="s">
+      <c r="H52">
+        <v>100</v>
+      </c>
+      <c r="I52" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="28.8">
+    <row r="53" spans="1:9" ht="28.8">
       <c r="A53" t="s">
         <v>220</v>
       </c>
@@ -3033,17 +2880,14 @@
       <c r="G53">
         <v>2</v>
       </c>
-      <c r="H53" t="s">
-        <v>222</v>
-      </c>
-      <c r="I53">
-        <v>100</v>
-      </c>
-      <c r="J53" t="s">
+      <c r="H53">
+        <v>100</v>
+      </c>
+      <c r="I53" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="28.8">
+    <row r="54" spans="1:9" ht="28.8">
       <c r="A54" t="s">
         <v>224</v>
       </c>
@@ -3065,17 +2909,14 @@
       <c r="G54">
         <v>2</v>
       </c>
-      <c r="H54" t="s">
-        <v>222</v>
-      </c>
-      <c r="I54">
-        <v>100</v>
-      </c>
-      <c r="J54" t="s">
+      <c r="H54">
+        <v>100</v>
+      </c>
+      <c r="I54" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>226</v>
       </c>
@@ -3097,35 +2938,320 @@
       <c r="G55">
         <v>2</v>
       </c>
-      <c r="H55" t="s">
-        <v>228</v>
-      </c>
-      <c r="I55">
-        <v>100</v>
-      </c>
-      <c r="J55" t="s">
+      <c r="H55">
+        <v>100</v>
+      </c>
+      <c r="I55" t="s">
         <v>285</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H112" xr:uid="{F4689175-1BCB-4AC3-A0ED-0BD6571DC856}"/>
-  <hyperlinks>
-    <hyperlink ref="H39" r:id="rId1" xr:uid="{EE71B5EC-E6F2-684B-8E1A-3C225CAF095B}"/>
-    <hyperlink ref="H43" r:id="rId2" xr:uid="{F8EB34A0-673C-FC44-B052-02E83C9FA7F3}"/>
-    <hyperlink ref="H2" r:id="rId3" xr:uid="{2DB111FE-06E9-4897-9F88-6732E0C6158D}"/>
-    <hyperlink ref="H3" r:id="rId4" xr:uid="{87A2F6D0-7C97-4E98-B519-22254F6818E0}"/>
-    <hyperlink ref="H4" r:id="rId5" xr:uid="{8109C618-3CD6-4025-93BC-4DC2CABB1DB6}"/>
-    <hyperlink ref="H5" r:id="rId6" xr:uid="{EB4D6E0C-DF31-4689-BCF4-FFC2CC5B0053}"/>
-    <hyperlink ref="H9" r:id="rId7" xr:uid="{EFBF34F6-0C22-44DF-9488-2824D1886503}"/>
-    <hyperlink ref="H10" r:id="rId8" xr:uid="{74E96DB0-BD87-457F-8CC2-83025A674B91}"/>
-    <hyperlink ref="H14" r:id="rId9" xr:uid="{35F2C76E-7145-4FFF-8550-5CD6A8C28B3B}"/>
-  </hyperlinks>
+  <autoFilter ref="A1:G112" xr:uid="{F4689175-1BCB-4AC3-A0ED-0BD6571DC856}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5CAA8C-9394-469B-8912-A26CF211B13A}">
+  <dimension ref="A1:A55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A39" r:id="rId1" xr:uid="{0C889494-5015-48E9-8CE7-53CED17C0F3F}"/>
+    <hyperlink ref="A43" r:id="rId2" xr:uid="{EB580A7A-2CC8-4526-9498-610868CE990A}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{36F9A532-095F-4F0A-981D-4A259D2B3E41}"/>
+    <hyperlink ref="A3" r:id="rId4" xr:uid="{FEDB8194-25A9-4587-978D-6335ADE11D70}"/>
+    <hyperlink ref="A4" r:id="rId5" xr:uid="{4B416753-A29B-46D9-8251-5767CC90B8D3}"/>
+    <hyperlink ref="A5" r:id="rId6" xr:uid="{06634815-E092-4BB3-8ADB-5274DCF30080}"/>
+    <hyperlink ref="A9" r:id="rId7" xr:uid="{3DCF78F9-D58C-4EB2-A473-6F9F7E98DDFA}"/>
+    <hyperlink ref="A10" r:id="rId8" xr:uid="{8156E5F0-0743-4384-BCE4-2A88CCB7C9A2}"/>
+    <hyperlink ref="A14" r:id="rId9" xr:uid="{A18CBA1B-E968-4B36-A167-B12BE07E75AB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C692A3D1-203D-4B7A-A3A3-8FE791B5F68C}">
   <dimension ref="A1:G18"/>
   <sheetViews>
@@ -3518,7 +3644,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABC0790-DD4E-4ACA-9441-7EACF1C3FF33}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -3568,7 +3694,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941B0DC6-BDCE-41B9-A5F1-4DF4C588FE69}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3580,7 +3706,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2525ABCD-A25A-478D-8461-E018B0A4DAA0}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3592,7 +3718,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{859F886B-DAD9-4B70-BD92-653B1D4E3565}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Change to delisting of product when "deleting it" on backend
</commit_message>
<xml_diff>
--- a/flask_project/data/awae_products.xlsx
+++ b/flask_project/data/awae_products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HDD documents\University\comp3900\capstone-project-3900-h10a-awae\flask_project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acidi\Coding\capstone-project-3900-h10a-awae\flask_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA368B2D-FA45-4696-81CB-F9E72BBFF948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67F6EB0-E7BE-44DF-8181-281F51BA6EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2064" yWindow="3576" windowWidth="18780" windowHeight="11976" xr2:uid="{D399C2E0-3F7A-4710-BFC9-FE24D65D8127}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D399C2E0-3F7A-4710-BFC9-FE24D65D8127}"/>
   </bookViews>
   <sheets>
     <sheet name="All Products" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="287">
   <si>
     <t>UID</t>
   </si>
@@ -950,12 +950,15 @@
   <si>
     <t>/static/uploads/images/54.png</t>
   </si>
+  <si>
+    <t>is_deleted</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1331,26 +1334,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4689175-1BCB-4AC3-A0ED-0BD6571DC856}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="85.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.109375" customWidth="1"/>
-    <col min="9" max="9" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="85.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1378,8 +1381,11 @@
       <c r="I1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="83.4" customHeight="1">
+      <c r="J1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1407,8 +1413,11 @@
       <c r="I2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="57.6">
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1436,8 +1445,11 @@
       <c r="I3" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="57.6">
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1465,8 +1477,11 @@
       <c r="I4" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="28.8">
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1494,8 +1509,11 @@
       <c r="I5" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="28.8">
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1523,8 +1541,11 @@
       <c r="I6" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="43.2">
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1552,8 +1573,11 @@
       <c r="I7" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="43.2">
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1581,8 +1605,11 @@
       <c r="I8" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="57.6">
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -1610,8 +1637,11 @@
       <c r="I9" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="43.2">
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1639,8 +1669,11 @@
       <c r="I10" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="25.8">
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -1668,8 +1701,11 @@
       <c r="I11" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="43.2">
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -1697,8 +1733,11 @@
       <c r="I12" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="43.2">
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -1726,8 +1765,11 @@
       <c r="I13" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="43.2">
+      <c r="J13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1755,8 +1797,11 @@
       <c r="I14" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="57.6">
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>78</v>
       </c>
@@ -1784,8 +1829,11 @@
       <c r="I15" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="28.8">
+      <c r="J15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -1813,8 +1861,11 @@
       <c r="I16" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="28.8">
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -1842,8 +1893,11 @@
       <c r="I17" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="28.8">
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>90</v>
       </c>
@@ -1871,8 +1925,11 @@
       <c r="I18" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="57.6">
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>95</v>
       </c>
@@ -1900,8 +1957,11 @@
       <c r="I19" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="129.6">
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>103</v>
       </c>
@@ -1929,8 +1989,11 @@
       <c r="I20" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="129.6">
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>107</v>
       </c>
@@ -1958,8 +2021,11 @@
       <c r="I21" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="129.6">
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>111</v>
       </c>
@@ -1987,8 +2053,11 @@
       <c r="I22" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="100.8">
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>113</v>
       </c>
@@ -2016,8 +2085,11 @@
       <c r="I23" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="43.2">
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -2045,8 +2117,11 @@
       <c r="I24" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="28.8">
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>124</v>
       </c>
@@ -2074,8 +2149,11 @@
       <c r="I25" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="28.8">
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -2103,8 +2181,11 @@
       <c r="I26" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="28.8">
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -2132,8 +2213,11 @@
       <c r="I27" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="57.6">
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>130</v>
       </c>
@@ -2161,8 +2245,11 @@
       <c r="I28" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="85.8" customHeight="1">
+      <c r="J28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="85.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>136</v>
       </c>
@@ -2190,8 +2277,11 @@
       <c r="I29" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="28.8">
+      <c r="J29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>139</v>
       </c>
@@ -2219,8 +2309,11 @@
       <c r="I30" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="43.2">
+      <c r="J30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>142</v>
       </c>
@@ -2248,8 +2341,11 @@
       <c r="I31" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>146</v>
       </c>
@@ -2277,8 +2373,11 @@
       <c r="I32" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="J32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>149</v>
       </c>
@@ -2306,8 +2405,11 @@
       <c r="I33" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>152</v>
       </c>
@@ -2335,8 +2437,11 @@
       <c r="I34" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>155</v>
       </c>
@@ -2364,8 +2469,11 @@
       <c r="I35" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="43.2">
+      <c r="J35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>161</v>
       </c>
@@ -2393,8 +2501,11 @@
       <c r="I36" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="43.2">
+      <c r="J36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>163</v>
       </c>
@@ -2422,8 +2533,11 @@
       <c r="I37" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="43.2">
+      <c r="J37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>168</v>
       </c>
@@ -2451,8 +2565,11 @@
       <c r="I38" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="28.8">
+      <c r="J38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>171</v>
       </c>
@@ -2480,8 +2597,11 @@
       <c r="I39" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="100.8">
+      <c r="J39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>174</v>
       </c>
@@ -2509,8 +2629,11 @@
       <c r="I40" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="43.2">
+      <c r="J40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>178</v>
       </c>
@@ -2538,8 +2661,11 @@
       <c r="I41" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="43.2">
+      <c r="J41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>181</v>
       </c>
@@ -2567,8 +2693,11 @@
       <c r="I42" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="57.6">
+      <c r="J42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>185</v>
       </c>
@@ -2596,8 +2725,11 @@
       <c r="I43" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="72">
+      <c r="J43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>189</v>
       </c>
@@ -2625,8 +2757,11 @@
       <c r="I44" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="57.6">
+      <c r="J44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>193</v>
       </c>
@@ -2654,8 +2789,11 @@
       <c r="I45" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="43.2">
+      <c r="J45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>197</v>
       </c>
@@ -2683,8 +2821,11 @@
       <c r="I46" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="57.6">
+      <c r="J46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>201</v>
       </c>
@@ -2712,8 +2853,11 @@
       <c r="I47" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="28.8">
+      <c r="J47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>205</v>
       </c>
@@ -2741,8 +2885,11 @@
       <c r="I48" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="J48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>209</v>
       </c>
@@ -2770,8 +2917,11 @@
       <c r="I49" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="28.8">
+      <c r="J49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>211</v>
       </c>
@@ -2799,8 +2949,11 @@
       <c r="I50" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="J50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>213</v>
       </c>
@@ -2828,8 +2981,11 @@
       <c r="I51" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="28.8">
+      <c r="J51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>216</v>
       </c>
@@ -2857,8 +3013,11 @@
       <c r="I52" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="28.8">
+      <c r="J52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>220</v>
       </c>
@@ -2886,8 +3045,11 @@
       <c r="I53" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="28.8">
+      <c r="J53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>224</v>
       </c>
@@ -2915,8 +3077,11 @@
       <c r="I54" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="J54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>226</v>
       </c>
@@ -2943,6 +3108,9 @@
       </c>
       <c r="I55" t="s">
         <v>285</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2960,277 +3128,277 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>228</v>
       </c>
@@ -3259,15 +3427,15 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
-    <col min="5" max="5" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="52.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3290,7 +3458,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -3314,7 +3482,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -3338,7 +3506,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -3362,7 +3530,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -3386,7 +3554,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -3410,7 +3578,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -3428,7 +3596,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -3446,7 +3614,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -3464,7 +3632,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -3482,7 +3650,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1010</v>
       </c>
@@ -3500,7 +3668,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1011</v>
       </c>
@@ -3518,7 +3686,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1012</v>
       </c>
@@ -3536,7 +3704,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1013</v>
       </c>
@@ -3554,7 +3722,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1014</v>
       </c>
@@ -3572,7 +3740,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1015</v>
       </c>
@@ -3593,7 +3761,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1016</v>
       </c>
@@ -3617,7 +3785,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1017</v>
       </c>
@@ -3652,9 +3820,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3665,7 +3833,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1018</v>
       </c>
@@ -3673,7 +3841,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1019</v>
       </c>
@@ -3681,7 +3849,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1020</v>
       </c>
@@ -3700,7 +3868,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3712,7 +3880,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3726,7 +3894,7 @@
       <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>